<commit_message>
changed to merge LA names rather than replace
</commit_message>
<xml_diff>
--- a/to_restructure.xlsx
+++ b/to_restructure.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\jcaddick\github\restructuring\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\jcaddick\github\la_restructuring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD56E809-59D1-4FA1-8002-3A07EECEF2C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63BC8264-E788-4D66-AE5C-CD85BEC0E86F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="30960" windowHeight="15570" xr2:uid="{2F2DD3A5-512E-492F-8932-BE175330B20B}"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="22770" windowHeight="13335" xr2:uid="{2F2DD3A5-512E-492F-8932-BE175330B20B}"/>
   </bookViews>
   <sheets>
     <sheet name="la structure" sheetId="1" r:id="rId1"/>
@@ -3496,7 +3496,7 @@
     <t>authority</t>
   </si>
   <si>
-    <t>class</t>
+    <t>la_class</t>
   </si>
 </sst>
 </file>
@@ -3863,7 +3863,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I9" sqref="I9"/>
+      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>